<commit_message>
Regras atualizadas e documentos atualizados
</commit_message>
<xml_diff>
--- a/Sistemas e Portais - SO I.xlsx
+++ b/Sistemas e Portais - SO I.xlsx
@@ -1,21 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/46679e56f61f2757/Documentos/Unesp/FPGA 2021_02/Recursos-ProjetoFPGA/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_F87197313802FFC3CFABA558C078A81B41AF77CE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FBC092CB-7133-49EA-A9E1-FDBD82835FB8}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sistemas e Portais - SO I" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="Card Deck 1" sheetId="2" r:id="rId4"/>
-    <sheet state="visible" name="Card Deck 2" sheetId="3" r:id="rId5"/>
-    <sheet state="visible" name="Materials" sheetId="4" r:id="rId6"/>
-    <sheet state="visible" name="Get the Link Here" sheetId="5" r:id="rId7"/>
+    <sheet name="Sistemas e Portais - SO I" sheetId="1" r:id="rId1"/>
+    <sheet name="Card Deck 1" sheetId="2" r:id="rId2"/>
+    <sheet name="Card Deck 2" sheetId="3" r:id="rId3"/>
+    <sheet name="Materials" sheetId="4" r:id="rId4"/>
+    <sheet name="Get the Link Here" sheetId="5" r:id="rId5"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="176">
   <si>
     <t>Space</t>
   </si>
@@ -619,92 +640,119 @@
   <si>
     <t>Template Version 3</t>
   </si>
+  <si>
+    <t>https://raw.githubusercontent.com/MajorMonge/Recursos-ProjetoFPGA/main/Regras%20-%20Sistemas%20e%20Portais.pdf</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dddd&quot;, &quot;mmmm&quot; &quot;d&quot;, &quot;yyyy&quot;, &quot;h&quot;:&quot;mm&quot;:&quot;ss&quot; &quot;am/pm"/>
+    <numFmt numFmtId="164" formatCode="dddd&quot;, &quot;mmmm&quot; &quot;d&quot;, &quot;yyyy&quot;, &quot;h&quot;:&quot;mm&quot;:&quot;ss&quot; &quot;AM/PM"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
-    </font>
-    <font>
-      <b/>
-      <color rgb="FF000000"/>
-    </font>
-    <font>
-      <b/>
-    </font>
-    <font/>
-    <font>
-      <b/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
       <u/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
       <u/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
       <i/>
+      <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
     </font>
     <font>
       <i/>
+      <sz val="10"/>
       <color rgb="FF666666"/>
       <name val="Arial"/>
     </font>
     <font>
       <i/>
       <u/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
       <i/>
-      <sz val="8.0"/>
+      <sz val="8"/>
       <color rgb="FF666666"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -713,7 +761,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -741,220 +789,482 @@
     </fill>
   </fills>
   <borders count="4">
-    <border/>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FFB7B7B7"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="50">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="0"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="8" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="8" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF6D9EEB"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="6.57"/>
-    <col customWidth="1" min="2" max="2" width="103.14"/>
-    <col customWidth="1" min="3" max="3" width="192.29"/>
+    <col min="1" max="1" width="6.5703125" customWidth="1"/>
+    <col min="2" max="2" width="103.140625" customWidth="1"/>
+    <col min="3" max="3" width="192.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -965,7 +1275,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -974,7 +1284,7 @@
       </c>
       <c r="C2" s="6"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
@@ -983,7 +1293,7 @@
       </c>
       <c r="C3" s="9"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
@@ -992,7 +1302,7 @@
       </c>
       <c r="C4" s="9"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -1001,7 +1311,7 @@
       </c>
       <c r="C5" s="9"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>11</v>
       </c>
@@ -1010,7 +1320,7 @@
       </c>
       <c r="C6" s="9"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>13</v>
       </c>
@@ -1019,7 +1329,7 @@
       </c>
       <c r="C7" s="9"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>14</v>
       </c>
@@ -1028,7 +1338,7 @@
       </c>
       <c r="C8" s="9"/>
     </row>
-    <row r="9" ht="18.75" customHeight="1">
+    <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>15</v>
       </c>
@@ -1039,7 +1349,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>18</v>
       </c>
@@ -1048,7 +1358,7 @@
       </c>
       <c r="C10" s="9"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>19</v>
       </c>
@@ -1057,7 +1367,7 @@
       </c>
       <c r="C11" s="9"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>20</v>
       </c>
@@ -1066,7 +1376,7 @@
       </c>
       <c r="C12" s="10"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>21</v>
       </c>
@@ -1075,7 +1385,7 @@
       </c>
       <c r="C13" s="9"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>22</v>
       </c>
@@ -1084,7 +1394,7 @@
       </c>
       <c r="C14" s="9"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>23</v>
       </c>
@@ -1093,7 +1403,7 @@
       </c>
       <c r="C15" s="11"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>24</v>
       </c>
@@ -1102,7 +1412,7 @@
       </c>
       <c r="C16" s="9"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>25</v>
       </c>
@@ -1111,7 +1421,7 @@
       </c>
       <c r="C17" s="9"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>26</v>
       </c>
@@ -1120,7 +1430,7 @@
       </c>
       <c r="C18" s="11"/>
     </row>
-    <row r="19" ht="18.75" customHeight="1">
+    <row r="19" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>27</v>
       </c>
@@ -1131,7 +1441,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>30</v>
       </c>
@@ -1140,7 +1450,7 @@
       </c>
       <c r="C20" s="11"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>31</v>
       </c>
@@ -1149,7 +1459,7 @@
       </c>
       <c r="C21" s="9"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>32</v>
       </c>
@@ -1158,7 +1468,7 @@
       </c>
       <c r="C22" s="9"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>33</v>
       </c>
@@ -1167,7 +1477,7 @@
       </c>
       <c r="C23" s="13"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>34</v>
       </c>
@@ -1176,7 +1486,7 @@
       </c>
       <c r="C24" s="9"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>35</v>
       </c>
@@ -1185,7 +1495,7 @@
       </c>
       <c r="C25" s="14"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>36</v>
       </c>
@@ -1194,7 +1504,7 @@
       </c>
       <c r="C26" s="11"/>
     </row>
-    <row r="27" ht="16.5" customHeight="1">
+    <row r="27" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>37</v>
       </c>
@@ -1205,7 +1515,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>40</v>
       </c>
@@ -1214,7 +1524,7 @@
       </c>
       <c r="C28" s="14"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>41</v>
       </c>
@@ -1223,7 +1533,7 @@
       </c>
       <c r="C29" s="9"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
         <v>42</v>
       </c>
@@ -1232,7 +1542,7 @@
       </c>
       <c r="C30" s="15"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>43</v>
       </c>
@@ -1241,7 +1551,7 @@
       </c>
       <c r="C31" s="9"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>44</v>
       </c>
@@ -1250,7 +1560,7 @@
       </c>
       <c r="C32" s="11"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
         <v>45</v>
       </c>
@@ -1259,7 +1569,7 @@
       </c>
       <c r="C33" s="16"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>46</v>
       </c>
@@ -1268,7 +1578,7 @@
       </c>
       <c r="C34" s="9"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="12" t="s">
         <v>47</v>
       </c>
@@ -1277,7 +1587,7 @@
       </c>
       <c r="C35" s="17"/>
     </row>
-    <row r="36" ht="12.75" customHeight="1">
+    <row r="36" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
         <v>48</v>
       </c>
@@ -1288,7 +1598,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>51</v>
       </c>
@@ -1297,7 +1607,7 @@
       </c>
       <c r="C37" s="9"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
         <v>52</v>
       </c>
@@ -1306,7 +1616,7 @@
       </c>
       <c r="C38" s="9"/>
     </row>
-    <row r="39">
+    <row r="39" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>53</v>
       </c>
@@ -1315,7 +1625,7 @@
       </c>
       <c r="C39" s="9"/>
     </row>
-    <row r="40">
+    <row r="40" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>54</v>
       </c>
@@ -1324,7 +1634,7 @@
       </c>
       <c r="C40" s="9"/>
     </row>
-    <row r="41">
+    <row r="41" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
         <v>55</v>
       </c>
@@ -1333,7 +1643,7 @@
       </c>
       <c r="C41" s="9"/>
     </row>
-    <row r="42">
+    <row r="42" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
         <v>56</v>
       </c>
@@ -1342,7 +1652,7 @@
       </c>
       <c r="C42" s="9"/>
     </row>
-    <row r="43">
+    <row r="43" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
         <v>57</v>
       </c>
@@ -1351,7 +1661,7 @@
       </c>
       <c r="C43" s="9"/>
     </row>
-    <row r="44">
+    <row r="44" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
         <v>58</v>
       </c>
@@ -1360,7 +1670,7 @@
       </c>
       <c r="C44" s="9"/>
     </row>
-    <row r="45">
+    <row r="45" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
         <v>59</v>
       </c>
@@ -1369,7 +1679,7 @@
       </c>
       <c r="C45" s="9"/>
     </row>
-    <row r="46">
+    <row r="46" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
         <v>60</v>
       </c>
@@ -1378,7 +1688,7 @@
       </c>
       <c r="C46" s="9"/>
     </row>
-    <row r="47">
+    <row r="47" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>61</v>
       </c>
@@ -1387,7 +1697,7 @@
       </c>
       <c r="C47" s="18"/>
     </row>
-    <row r="48">
+    <row r="48" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
         <v>62</v>
       </c>
@@ -1396,7 +1706,7 @@
       </c>
       <c r="C48" s="19"/>
     </row>
-    <row r="49">
+    <row r="49" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
         <v>64</v>
       </c>
@@ -1406,29 +1716,30 @@
       <c r="C49" s="19"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFD966"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="133.14"/>
-    <col customWidth="1" min="2" max="2" width="54.71"/>
+    <col min="1" max="1" width="133.140625" customWidth="1"/>
+    <col min="2" max="2" width="54.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
         <v>66</v>
       </c>
@@ -1436,312 +1747,313 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
         <v>68</v>
       </c>
       <c r="B2" s="23"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
         <v>69</v>
       </c>
       <c r="B3" s="24"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
         <v>70</v>
       </c>
       <c r="B4" s="25"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
         <v>71</v>
       </c>
       <c r="B5" s="24"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
         <v>72</v>
       </c>
       <c r="B6" s="24"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
         <v>73</v>
       </c>
       <c r="B7" s="23"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
         <v>74</v>
       </c>
       <c r="B8" s="26"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="22" t="s">
         <v>75</v>
       </c>
       <c r="B9" s="26"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="22" t="s">
         <v>76</v>
       </c>
       <c r="B10" s="26"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="22" t="s">
         <v>77</v>
       </c>
       <c r="B11" s="26"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="22" t="s">
         <v>78</v>
       </c>
       <c r="B12" s="26"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="22" t="s">
         <v>79</v>
       </c>
       <c r="B13" s="26"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="22" t="s">
         <v>80</v>
       </c>
       <c r="B14" s="26"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="22" t="s">
         <v>81</v>
       </c>
       <c r="B15" s="26"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="22" t="s">
         <v>82</v>
       </c>
       <c r="B16" s="27"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="22" t="s">
         <v>83</v>
       </c>
       <c r="B17" s="27"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="22" t="s">
         <v>84</v>
       </c>
       <c r="B18" s="28"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="22" t="s">
         <v>85</v>
       </c>
       <c r="B19" s="28"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="22" t="s">
         <v>86</v>
       </c>
       <c r="B20" s="27"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="22" t="s">
         <v>87</v>
       </c>
       <c r="B21" s="27"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="22" t="s">
         <v>88</v>
       </c>
       <c r="B22" s="27"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="22" t="s">
         <v>89</v>
       </c>
       <c r="B23" s="27"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="22" t="s">
         <v>90</v>
       </c>
       <c r="B24" s="27"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="22" t="s">
         <v>91</v>
       </c>
       <c r="B25" s="27"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="22" t="s">
         <v>92</v>
       </c>
       <c r="B26" s="27"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="22" t="s">
         <v>93</v>
       </c>
       <c r="B27" s="27"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="22" t="s">
         <v>94</v>
       </c>
       <c r="B28" s="27"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="22" t="s">
         <v>95</v>
       </c>
       <c r="B29" s="27"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="22" t="s">
         <v>96</v>
       </c>
       <c r="B30" s="27"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="22" t="s">
         <v>97</v>
       </c>
       <c r="B31" s="27"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="22" t="s">
         <v>98</v>
       </c>
       <c r="B32" s="27"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="22" t="s">
         <v>99</v>
       </c>
       <c r="B33" s="27"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="22" t="s">
         <v>100</v>
       </c>
       <c r="B34" s="27"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="22" t="s">
         <v>101</v>
       </c>
       <c r="B35" s="27"/>
     </row>
-    <row r="36">
+    <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="22" t="s">
         <v>102</v>
       </c>
       <c r="B36" s="27"/>
     </row>
-    <row r="37">
+    <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="22" t="s">
         <v>103</v>
       </c>
       <c r="B37" s="27"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="22" t="s">
         <v>104</v>
       </c>
       <c r="B38" s="27"/>
     </row>
-    <row r="39">
+    <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="22" t="s">
         <v>105</v>
       </c>
       <c r="B39" s="27"/>
     </row>
-    <row r="40">
+    <row r="40" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="22" t="s">
         <v>106</v>
       </c>
       <c r="B40" s="27"/>
     </row>
-    <row r="41">
+    <row r="41" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="22" t="s">
         <v>107</v>
       </c>
       <c r="B41" s="27"/>
     </row>
-    <row r="42">
+    <row r="42" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="22" t="s">
         <v>108</v>
       </c>
       <c r="B42" s="27"/>
     </row>
-    <row r="43">
+    <row r="43" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="22"/>
       <c r="B43" s="27"/>
     </row>
-    <row r="44">
+    <row r="44" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="22"/>
       <c r="B44" s="27"/>
     </row>
-    <row r="45">
+    <row r="45" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="22"/>
       <c r="B45" s="27"/>
     </row>
-    <row r="46">
+    <row r="46" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="22"/>
       <c r="B46" s="27"/>
     </row>
-    <row r="47">
+    <row r="47" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="22"/>
       <c r="B47" s="27"/>
     </row>
-    <row r="48">
+    <row r="48" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="22"/>
       <c r="B48" s="27"/>
     </row>
-    <row r="49">
+    <row r="49" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="22"/>
       <c r="B49" s="27"/>
     </row>
-    <row r="50">
+    <row r="50" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="22"/>
       <c r="B50" s="27"/>
     </row>
-    <row r="51">
+    <row r="51" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="22"/>
       <c r="B51" s="27"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFD966"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="193.86"/>
-    <col customWidth="1" min="2" max="2" width="54.71"/>
+    <col min="1" max="1" width="193.85546875" customWidth="1"/>
+    <col min="2" max="2" width="54.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>66</v>
       </c>
@@ -1749,272 +2061,273 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
         <v>109</v>
       </c>
       <c r="B2" s="24"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>110</v>
       </c>
       <c r="B3" s="16"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>39</v>
       </c>
       <c r="B4" s="16"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>111</v>
       </c>
       <c r="B5" s="16"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>112</v>
       </c>
       <c r="B6" s="16"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>113</v>
       </c>
       <c r="B7" s="16"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>114</v>
       </c>
       <c r="B8" s="23"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>115</v>
       </c>
       <c r="B9" s="26"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>116</v>
       </c>
       <c r="B10" s="26"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>117</v>
       </c>
       <c r="B11" s="26"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>118</v>
       </c>
       <c r="B12" s="26"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>119</v>
       </c>
       <c r="B13" s="26"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>120</v>
       </c>
       <c r="B14" s="26"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>119</v>
       </c>
       <c r="B15" s="26"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>120</v>
       </c>
       <c r="B16" s="27"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>120</v>
       </c>
       <c r="B17" s="27"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>111</v>
       </c>
       <c r="B18" s="28"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="24" t="s">
         <v>109</v>
       </c>
       <c r="B19" s="28"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
         <v>115</v>
       </c>
       <c r="B20" s="27"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
         <v>39</v>
       </c>
       <c r="B21" s="27"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>118</v>
       </c>
       <c r="B22" s="27"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="27"/>
       <c r="B23" s="27"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="27"/>
       <c r="B24" s="27"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="27"/>
       <c r="B25" s="27"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="27"/>
       <c r="B26" s="27"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="27"/>
       <c r="B27" s="27"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="27"/>
       <c r="B28" s="27"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="27"/>
       <c r="B29" s="27"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="27"/>
       <c r="B30" s="27"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="27"/>
       <c r="B31" s="27"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="27"/>
       <c r="B32" s="27"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="27"/>
       <c r="B33" s="27"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="27"/>
       <c r="B34" s="27"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="27"/>
       <c r="B35" s="27"/>
     </row>
-    <row r="36">
+    <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="27"/>
       <c r="B36" s="27"/>
     </row>
-    <row r="37">
+    <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="27"/>
       <c r="B37" s="27"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="27"/>
       <c r="B38" s="27"/>
     </row>
-    <row r="39">
+    <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="27"/>
       <c r="B39" s="27"/>
     </row>
-    <row r="40">
+    <row r="40" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="27"/>
       <c r="B40" s="27"/>
     </row>
-    <row r="41">
+    <row r="41" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="27"/>
       <c r="B41" s="27"/>
     </row>
-    <row r="42">
+    <row r="42" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="27"/>
       <c r="B42" s="27"/>
     </row>
-    <row r="43">
+    <row r="43" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="27"/>
       <c r="B43" s="27"/>
     </row>
-    <row r="44">
+    <row r="44" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="27"/>
       <c r="B44" s="27"/>
     </row>
-    <row r="45">
+    <row r="45" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="27"/>
       <c r="B45" s="27"/>
     </row>
-    <row r="46">
+    <row r="46" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="27"/>
       <c r="B46" s="27"/>
     </row>
-    <row r="47">
+    <row r="47" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="27"/>
       <c r="B47" s="27"/>
     </row>
-    <row r="48">
+    <row r="48" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="27"/>
       <c r="B48" s="27"/>
     </row>
-    <row r="49">
+    <row r="49" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="27"/>
       <c r="B49" s="27"/>
     </row>
-    <row r="50">
+    <row r="50" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="27"/>
       <c r="B50" s="27"/>
     </row>
-    <row r="51">
+    <row r="51" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="27"/>
       <c r="B51" s="27"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFD966"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="27.14"/>
-    <col customWidth="1" min="2" max="2" width="121.86"/>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="121.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>121</v>
       </c>
@@ -2022,7 +2335,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
         <v>123</v>
       </c>
@@ -2030,7 +2343,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="29" t="s">
         <v>125</v>
       </c>
@@ -2038,7 +2351,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="s">
         <v>127</v>
       </c>
@@ -2046,7 +2359,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
         <v>129</v>
       </c>
@@ -2054,7 +2367,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="29" t="s">
         <v>131</v>
       </c>
@@ -2062,7 +2375,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="29" t="s">
         <v>133</v>
       </c>
@@ -2070,19 +2383,19 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="29" t="s">
         <v>135</v>
       </c>
       <c r="B8" s="31"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
         <v>136</v>
       </c>
       <c r="B9" s="33"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="29" t="s">
         <v>137</v>
       </c>
@@ -2090,7 +2403,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="29" t="s">
         <v>139</v>
       </c>
@@ -2098,7 +2411,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="29" t="s">
         <v>141</v>
       </c>
@@ -2106,7 +2419,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="29" t="s">
         <v>143</v>
       </c>
@@ -2114,7 +2427,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="29" t="s">
         <v>145</v>
       </c>
@@ -2122,7 +2435,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="32" t="s">
         <v>147</v>
       </c>
@@ -2130,79 +2443,79 @@
         <v>148</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="29" t="s">
         <v>149</v>
       </c>
       <c r="B16" s="34"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="29" t="s">
         <v>150</v>
       </c>
       <c r="B17" s="34"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="29" t="s">
         <v>151</v>
       </c>
       <c r="B18" s="34"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="29" t="s">
         <v>152</v>
       </c>
       <c r="B19" s="34"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="29" t="s">
         <v>153</v>
       </c>
       <c r="B20" s="34"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="32" t="s">
         <v>154</v>
       </c>
       <c r="B21" s="35"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="29" t="s">
         <v>155</v>
       </c>
       <c r="B22" s="31"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="29" t="s">
         <v>156</v>
       </c>
       <c r="B23" s="31"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="29" t="s">
         <v>157</v>
       </c>
       <c r="B24" s="31"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="29" t="s">
         <v>158</v>
       </c>
       <c r="B25" s="31"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="29" t="s">
         <v>159</v>
       </c>
       <c r="B26" s="31"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="32" t="s">
         <v>160</v>
       </c>
       <c r="B27" s="33"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="29" t="s">
         <v>161</v>
       </c>
@@ -2210,7 +2523,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="29" t="s">
         <v>163</v>
       </c>
@@ -2218,7 +2531,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="29" t="s">
         <v>165</v>
       </c>
@@ -2226,7 +2539,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="32" t="s">
         <v>166</v>
       </c>
@@ -2234,13 +2547,15 @@
         <v>167</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="29" t="s">
         <v>168</v>
       </c>
-      <c r="B32" s="30"/>
-    </row>
-    <row r="33">
+      <c r="B32" s="49" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="37" t="s">
         <v>169</v>
       </c>
@@ -2249,206 +2564,208 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="B33">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" sqref="B33" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"Libre Franklin,Tinos,Balsamiq Sans,Poppins"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
-    <hyperlink r:id="rId2" ref="B3"/>
-    <hyperlink r:id="rId3" ref="B4"/>
-    <hyperlink r:id="rId4" ref="B5"/>
-    <hyperlink r:id="rId5" ref="B6"/>
-    <hyperlink r:id="rId6" ref="B7"/>
-    <hyperlink r:id="rId7" ref="B29"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink ref="B29" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
+    <hyperlink ref="B32" r:id="rId8" xr:uid="{F578076F-1995-4040-A348-D85D86E13D8C}"/>
   </hyperlinks>
-  <drawing r:id="rId8"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FF93C47D"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:A50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="137.57"/>
+    <col min="1" max="1" width="137.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="39" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="2" ht="33.0" customHeight="1">
+    <row r="2" spans="1:1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="40" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("IF(A8="""",HYPERLINK(""https://www.flippity.net/bg.php?k="" &amp; getId(),""https://www.flippity.net/bg.php?k="" &amp; getId() &amp; SUBSTITUTE(A3,A3,"""")),HYPERLINK(""https://www.flippity.net/bg.php?k="" &amp; REGEXEXTRACT(A8,""/d/(.*)/edit""),""https://www.flippity.ne"&amp;"t/bg.php?k="" &amp; REGEXEXTRACT(A8,""/d/(.*)/edit"")))"),"https://www.flippity.net/bg.php?k=1SNIg4RjCWFvH9hPnjXxswn9J0_JyDW1y2dSriDEJdPU")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("IF(A8="""",HYPERLINK(""https://www.flippity.net/bg.php?k="" &amp; getId(),""https://www.flippity.net/bg.php?k="" &amp; getId() &amp; SUBSTITUTE(A3,A3,"""")),HYPERLINK(""https://www.flippity.net/bg.php?k="" &amp; REGEXEXTRACT(A8,""/d/(.*)/edit""),""https://www.flippity.ne"&amp;"t/bg.php?k="" &amp; REGEXEXTRACT(A8,""/d/(.*)/edit"")))"),"https://www.flippity.net/bg.php?k=1SNIg4RjCWFvH9hPnjXxswn9J0_JyDW1y2dSriDEJdPU")</f>
         <v>https://www.flippity.net/bg.php?k=1SNIg4RjCWFvH9hPnjXxswn9J0_JyDW1y2dSriDEJdPU</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="41">
-        <f>now()</f>
-        <v>44612.88986</v>
-      </c>
-    </row>
-    <row r="4">
+        <f ca="1">NOW()</f>
+        <v>44627.990868981484</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="42" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="43" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="44" t="str">
         <f>HYPERLINK("http://www.flippity.net/Troubleshooting.asp","See Troubleshooting for more help.")</f>
         <v>See Troubleshooting for more help.</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="45"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="46"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="47"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="48" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="47"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="47"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="47"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="47"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="47"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="47"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="47"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="47"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="47"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="47"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="47"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="47"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="47"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="47"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="47"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="47"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="47"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="47"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="47"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="47"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="47"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="47"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="47"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="47"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="47"/>
     </row>
-    <row r="36">
+    <row r="36" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="47"/>
     </row>
-    <row r="37">
+    <row r="37" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="47"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="47"/>
     </row>
-    <row r="39">
+    <row r="39" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="47"/>
     </row>
-    <row r="40">
+    <row r="40" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="47"/>
     </row>
-    <row r="41">
+    <row r="41" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="47"/>
     </row>
-    <row r="42">
+    <row r="42" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="47"/>
     </row>
-    <row r="43">
+    <row r="43" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="47"/>
     </row>
-    <row r="44">
+    <row r="44" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="47"/>
     </row>
-    <row r="45">
+    <row r="45" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="47"/>
     </row>
-    <row r="46">
+    <row r="46" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="47"/>
     </row>
-    <row r="47">
+    <row r="47" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="47"/>
     </row>
-    <row r="48">
+    <row r="48" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="47"/>
     </row>
-    <row r="49">
+    <row r="49" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="47"/>
     </row>
-    <row r="50">
+    <row r="50" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="47"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>